<commit_message>
Alterações na leitura de dados
</commit_message>
<xml_diff>
--- a/tests/testesmanuais/CBA_SESI_Planilha_Dados_Entrada_Iniciativas - v0.3.xlsx
+++ b/tests/testesmanuais/CBA_SESI_Planilha_Dados_Entrada_Iniciativas - v0.3.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="8175" tabRatio="892" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12120" windowHeight="8175" tabRatio="892" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pl. suporte" sheetId="51" state="hidden" r:id="rId1"/>
@@ -484,12 +484,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -747,7 +747,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -986,14 +986,29 @@
     <xf numFmtId="10" fontId="2" fillId="3" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="9" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1007,32 +1022,17 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="Moeda 2" xfId="4"/>
+    <cellStyle name="Moeda 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="6" builtinId="5"/>
-    <cellStyle name="Vírgula 2" xfId="1"/>
-    <cellStyle name="Vírgula 2 2" xfId="2"/>
-    <cellStyle name="Vírgula 2 3" xfId="8"/>
-    <cellStyle name="Vírgula 3" xfId="5"/>
-    <cellStyle name="Vírgula 4" xfId="3"/>
-    <cellStyle name="Vírgula 5" xfId="7"/>
+    <cellStyle name="Vírgula 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Vírgula 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Vírgula 2 3" xfId="8" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Vírgula 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Vírgula 4" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Vírgula 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1409,7 +1409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1522,7 +1522,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -1818,18 +1818,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -1839,65 +1839,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -1910,17 +1910,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -2736,20 +2736,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -2970,20 +2970,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -3226,11 +3226,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -3247,11 +3247,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3259,7 +3259,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -3555,18 +3555,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -3576,65 +3576,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -3647,17 +3647,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -4473,20 +4473,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -4707,20 +4707,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -4963,11 +4963,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -4984,11 +4984,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4996,7 +4996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -5292,18 +5292,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -5313,65 +5313,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -5384,17 +5384,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -6210,20 +6210,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -6444,20 +6444,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -6700,11 +6700,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -6721,11 +6721,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6733,7 +6733,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -7029,18 +7029,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -7050,65 +7050,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -7121,17 +7121,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -7947,20 +7947,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -8181,20 +8181,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -8437,11 +8437,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -8458,11 +8458,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8470,7 +8470,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF7574"/>
   </sheetPr>
@@ -8667,19 +8667,19 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>'Pl. suporte'!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>D13:D21</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>'Pl. suporte'!$B$2:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>C7</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'Pl. suporte'!$C$2:$C$11</xm:f>
           </x14:formula1>
@@ -8692,7 +8692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF7574"/>
   </sheetPr>
@@ -9177,7 +9177,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -9462,18 +9462,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -9483,65 +9483,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="79" t="s">
         <v>71</v>
       </c>
@@ -9554,17 +9554,17 @@
       <c r="F17" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -10390,20 +10390,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -10664,20 +10664,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -10947,6 +10947,24 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:H39"/>
+    <mergeCell ref="I39:K39"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="L16:L17"/>
     <mergeCell ref="M16:M17"/>
@@ -10955,24 +10973,6 @@
     <mergeCell ref="O16:O17"/>
     <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="I15:K15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:H39"/>
-    <mergeCell ref="I39:K39"/>
-    <mergeCell ref="I50:K50"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10983,7 +10983,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -11261,18 +11261,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -11282,65 +11282,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -11353,17 +11353,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -12193,20 +12193,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -12466,20 +12466,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -12750,11 +12750,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -12771,11 +12771,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -12786,7 +12786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -13073,18 +13073,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -13094,65 +13094,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -13165,17 +13165,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -14004,20 +14004,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -14278,20 +14278,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -14558,11 +14558,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -14579,11 +14579,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -14594,7 +14594,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -14890,18 +14890,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -14911,65 +14911,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -14982,17 +14982,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -15822,20 +15822,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -16056,20 +16056,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -16312,11 +16312,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -16333,11 +16333,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16348,7 +16348,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -16644,18 +16644,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -16665,65 +16665,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -16736,17 +16736,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -17562,20 +17562,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -17796,20 +17796,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -18052,11 +18052,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -18073,11 +18073,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18085,7 +18085,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFCBC77"/>
   </sheetPr>
@@ -18381,18 +18381,18 @@
       <c r="N13" s="22"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="97" t="s">
+      <c r="A15" s="93" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="98" t="s">
+      <c r="C15" s="94" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="98"/>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
       <c r="G15" s="95" t="s">
         <v>51</v>
       </c>
@@ -18402,65 +18402,65 @@
       </c>
       <c r="J15" s="95"/>
       <c r="K15" s="95"/>
-      <c r="L15" s="99" t="s">
+      <c r="L15" s="91" t="s">
         <v>98</v>
       </c>
-      <c r="M15" s="99"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99" t="s">
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="99"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
     </row>
     <row r="16" spans="1:17" s="17" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="96"/>
-      <c r="C16" s="96" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="96"/>
-      <c r="E16" s="96" t="s">
+      <c r="D16" s="92"/>
+      <c r="E16" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="96"/>
-      <c r="G16" s="96" t="s">
+      <c r="F16" s="92"/>
+      <c r="G16" s="92" t="s">
         <v>48</v>
       </c>
-      <c r="H16" s="96" t="s">
+      <c r="H16" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="92" t="s">
         <v>73</v>
       </c>
-      <c r="J16" s="96" t="s">
+      <c r="J16" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="K16" s="96" t="s">
+      <c r="K16" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="L16" s="96" t="s">
+      <c r="L16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="96" t="s">
+      <c r="M16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="N16" s="96" t="s">
+      <c r="N16" s="92" t="s">
         <v>7</v>
       </c>
-      <c r="O16" s="96" t="s">
+      <c r="O16" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="96" t="s">
+      <c r="P16" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="Q16" s="96" t="s">
+      <c r="Q16" s="92" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:17" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="96"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="81" t="s">
         <v>71</v>
       </c>
@@ -18473,17 +18473,17 @@
       <c r="F17" s="81" t="s">
         <v>47</v>
       </c>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="96"/>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="96"/>
-      <c r="O17" s="96"/>
-      <c r="P17" s="96"/>
-      <c r="Q17" s="96"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="92"/>
+      <c r="I17" s="92"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="92"/>
+      <c r="M17" s="92"/>
+      <c r="N17" s="92"/>
+      <c r="O17" s="92"/>
+      <c r="P17" s="92"/>
+      <c r="Q17" s="92"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
@@ -19299,20 +19299,20 @@
       <c r="N38" s="2"/>
     </row>
     <row r="39" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="94" t="s">
+      <c r="E39" s="97"/>
+      <c r="F39" s="99" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93" t="s">
+      <c r="G39" s="98"/>
+      <c r="H39" s="98"/>
+      <c r="I39" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J39" s="93"/>
-      <c r="K39" s="93"/>
+      <c r="J39" s="98"/>
+      <c r="K39" s="98"/>
       <c r="L39" s="34" t="s">
         <v>21</v>
       </c>
@@ -19533,20 +19533,20 @@
       <c r="N49" s="2"/>
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="96" t="s">
         <v>97</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="93" t="s">
+      <c r="E50" s="97"/>
+      <c r="F50" s="98" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="93"/>
-      <c r="H50" s="93"/>
-      <c r="I50" s="93" t="s">
+      <c r="G50" s="98"/>
+      <c r="H50" s="98"/>
+      <c r="I50" s="98" t="s">
         <v>52</v>
       </c>
-      <c r="J50" s="93"/>
-      <c r="K50" s="93"/>
+      <c r="J50" s="98"/>
+      <c r="K50" s="98"/>
       <c r="L50" s="34" t="s">
         <v>21</v>
       </c>
@@ -19789,11 +19789,11 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="I15:K15"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="F50:H50"/>
+    <mergeCell ref="I50:K50"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
     <mergeCell ref="Q16:Q17"/>
     <mergeCell ref="D39:E39"/>
     <mergeCell ref="F39:H39"/>
@@ -19810,11 +19810,11 @@
     <mergeCell ref="M16:M17"/>
     <mergeCell ref="L15:N15"/>
     <mergeCell ref="N16:N17"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="F50:H50"/>
-    <mergeCell ref="I50:K50"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="I15:K15"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>